<commit_message>
total plus logic-Still error
</commit_message>
<xml_diff>
--- a/Excel/trip_3_13.xlsx
+++ b/Excel/trip_3_13.xlsx
@@ -2852,12 +2852,18 @@
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
+      <c r="F8" s="35">
+        <v>42320.0</v>
+      </c>
+      <c r="G8" s="36">
+        <v>42321.0</v>
+      </c>
+      <c r="H8" s="36">
+        <v>42322.0</v>
+      </c>
+      <c r="I8" s="36">
+        <v>42327.0</v>
+      </c>
       <c r="J8" s="36"/>
       <c r="K8" s="36"/>
       <c r="L8" s="36"/>
@@ -2902,16 +2908,20 @@
         <v>28</v>
       </c>
       <c r="E10" s="43"/>
-      <c r="F10" s="44"/>
+      <c r="F10" s="44">
+        <v>1.0</v>
+      </c>
       <c r="G10" s="44"/>
       <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
+      <c r="I10" s="44">
+        <v>12.0</v>
+      </c>
       <c r="J10" s="44"/>
       <c r="K10" s="44"/>
       <c r="L10" s="44"/>
-      <c r="M10" s="45" t="n">
+      <c r="M10" s="45">
         <f aca="false">SUM(F10:L10)</f>
-        <v>0</v>
+        <v>13.0</v>
       </c>
       <c r="N10" s="0"/>
       <c r="P10" s="0"/>
@@ -2927,16 +2937,18 @@
         <v>30</v>
       </c>
       <c r="E11" s="43"/>
-      <c r="F11" s="44"/>
+      <c r="F11" s="44">
+        <v>2.0</v>
+      </c>
       <c r="G11" s="44"/>
       <c r="H11" s="44"/>
       <c r="I11" s="44"/>
       <c r="J11" s="44"/>
       <c r="K11" s="44"/>
       <c r="L11" s="44"/>
-      <c r="M11" s="45" t="n">
+      <c r="M11" s="45">
         <f aca="false">SUM(F11:L11)</f>
-        <v>0</v>
+        <v>2.0</v>
       </c>
       <c r="N11" s="0"/>
       <c r="P11" s="0"/>
@@ -2953,15 +2965,17 @@
       </c>
       <c r="E12" s="43"/>
       <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
+      <c r="G12" s="44">
+        <v>11.0</v>
+      </c>
       <c r="H12" s="44"/>
       <c r="I12" s="44"/>
       <c r="J12" s="44"/>
       <c r="K12" s="44"/>
       <c r="L12" s="44"/>
-      <c r="M12" s="45" t="n">
+      <c r="M12" s="45">
         <f aca="false">SUM(F12:L12)</f>
-        <v>0</v>
+        <v>11.0</v>
       </c>
       <c r="N12" s="0"/>
       <c r="P12" s="0"/>
@@ -3003,7 +3017,9 @@
         <f aca="false">SUM(L10:L12)</f>
         <v>0</v>
       </c>
-      <c r="M13" s="49"/>
+      <c r="M13" s="49">
+        <v>0</v>
+      </c>
       <c r="N13" s="0"/>
       <c r="P13" s="0"/>
       <c r="Q13" s="0"/>
@@ -3025,7 +3041,7 @@
       <c r="J14" s="51"/>
       <c r="K14" s="51"/>
       <c r="L14" s="51"/>
-      <c r="M14" s="45" t="n">
+      <c r="M14" s="45">
         <f aca="false">SUM(F14:L14)</f>
         <v>0</v>
       </c>
@@ -3048,9 +3064,9 @@
       <c r="J15" s="52"/>
       <c r="K15" s="52"/>
       <c r="L15" s="52"/>
-      <c r="M15" s="53" t="n">
+      <c r="M15" s="53">
         <f aca="false">IF(M4="Y",SUM(M10:M14,'Page 2'!M15,'Page 3'!M15),SUM(M10:M14))</f>
-        <v>0</v>
+        <v>26.0</v>
       </c>
       <c r="N15" s="0"/>
       <c r="P15" s="0"/>
@@ -3073,7 +3089,7 @@
       <c r="J16" s="44"/>
       <c r="K16" s="44"/>
       <c r="L16" s="44"/>
-      <c r="M16" s="45" t="n">
+      <c r="M16" s="45">
         <f aca="false">SUM(F16:L16)</f>
         <v>0</v>
       </c>
@@ -3093,14 +3109,16 @@
       <c r="E17" s="43"/>
       <c r="F17" s="44"/>
       <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
+      <c r="H17" s="44">
+        <v>22.0</v>
+      </c>
       <c r="I17" s="44"/>
       <c r="J17" s="44"/>
       <c r="K17" s="44"/>
       <c r="L17" s="44"/>
-      <c r="M17" s="45" t="n">
+      <c r="M17" s="45">
         <f aca="false">SUM(F17:L17)</f>
-        <v>0</v>
+        <v>22.0</v>
       </c>
       <c r="N17" s="0"/>
       <c r="P17" s="0"/>
@@ -3118,14 +3136,16 @@
       <c r="E18" s="43"/>
       <c r="F18" s="44"/>
       <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
+      <c r="H18" s="44">
+        <v>222.0</v>
+      </c>
       <c r="I18" s="44"/>
       <c r="J18" s="44"/>
       <c r="K18" s="44"/>
       <c r="L18" s="44"/>
-      <c r="M18" s="45" t="n">
+      <c r="M18" s="45">
         <f aca="false">SUM(F18:L18)</f>
-        <v>0</v>
+        <v>222.0</v>
       </c>
       <c r="N18" s="0"/>
       <c r="P18" s="0"/>
@@ -3148,7 +3168,7 @@
       <c r="J19" s="44"/>
       <c r="K19" s="44"/>
       <c r="L19" s="44"/>
-      <c r="M19" s="55" t="n">
+      <c r="M19" s="55">
         <f aca="false">SUM(F19:L19)</f>
         <v>0</v>
       </c>
@@ -3173,7 +3193,7 @@
       <c r="J20" s="44"/>
       <c r="K20" s="44"/>
       <c r="L20" s="44"/>
-      <c r="M20" s="45" t="n">
+      <c r="M20" s="45">
         <f aca="false">SUM(F20:L20)</f>
         <v>0</v>
       </c>
@@ -3196,9 +3216,9 @@
       <c r="J21" s="56"/>
       <c r="K21" s="56"/>
       <c r="L21" s="56"/>
-      <c r="M21" s="57" t="n">
+      <c r="M21" s="57">
         <f aca="false">IF(M4="Y",SUM(M16:M20,'Page 2'!M21,'Page 3'!M21),SUM(M16:M20))</f>
-        <v>0</v>
+        <v>244.0</v>
       </c>
       <c r="N21" s="0"/>
       <c r="P21" s="0"/>
@@ -3269,18 +3289,30 @@
       </c>
       <c r="C24" s="71"/>
       <c r="D24" s="72"/>
-      <c r="E24" s="73"/>
+      <c r="E24" s="73" t="str">
+        <v>sa</v>
+      </c>
       <c r="F24" s="73"/>
-      <c r="G24" s="73"/>
+      <c r="G24" s="73" t="str">
+        <v>sa</v>
+      </c>
       <c r="H24" s="73"/>
-      <c r="I24" s="74"/>
-      <c r="J24" s="75" t="n">
+      <c r="I24" s="74">
+        <v>1</v>
+      </c>
+      <c r="J24" s="75">
         <f aca="false">IF(C24="C",(I24*0.3),IF(AND(D24&gt;=DATE(2015,1,1),D24&lt;=DATE(2015,12,31)),I24*0.575,IF(AND(D24&gt;=DATE(2016,1,1),D24&lt;=DATE(2016,12,31)),I24*0.54,IF(AND(D24&gt;=DATE(2017,1,1),D24&lt;=DATE(2017,12,31)),I24*0.535, I24*0))))</f>
-        <v>0</v>
-      </c>
-      <c r="K24" s="76"/>
-      <c r="L24" s="77"/>
-      <c r="M24" s="78"/>
+        <v>11.0</v>
+      </c>
+      <c r="K24" s="76">
+        <v>11.0</v>
+      </c>
+      <c r="L24" s="77">
+        <v>11.0</v>
+      </c>
+      <c r="M24" s="78">
+        <v>11.0</v>
+      </c>
       <c r="N24" s="79"/>
       <c r="P24" s="0"/>
       <c r="Q24" s="0"/>
@@ -3292,18 +3324,30 @@
       </c>
       <c r="C25" s="71"/>
       <c r="D25" s="72"/>
-      <c r="E25" s="73"/>
+      <c r="E25" s="73" t="str">
+        <v>1</v>
+      </c>
       <c r="F25" s="73"/>
-      <c r="G25" s="73"/>
+      <c r="G25" s="73" t="str">
+        <v>2</v>
+      </c>
       <c r="H25" s="73"/>
-      <c r="I25" s="74"/>
-      <c r="J25" s="75" t="n">
+      <c r="I25" s="74">
+        <v>2</v>
+      </c>
+      <c r="J25" s="75">
         <f aca="false">IF(C25="C",(I25*0.3),IF(AND(D25&gt;=DATE(2015,1,1),D25&lt;=DATE(2015,12,31)),I25*0.575,IF(AND(D25&gt;=DATE(2016,1,1),D25&lt;=DATE(2016,12,31)),I25*0.54,IF(AND(D25&gt;=DATE(2017,1,1),D25&lt;=DATE(2017,12,31)),I25*0.535, I25*0))))</f>
-        <v>0</v>
-      </c>
-      <c r="K25" s="76"/>
-      <c r="L25" s="81"/>
-      <c r="M25" s="82"/>
+        <v>22.0</v>
+      </c>
+      <c r="K25" s="76">
+        <v>22.0</v>
+      </c>
+      <c r="L25" s="81">
+        <v>22.0</v>
+      </c>
+      <c r="M25" s="82">
+        <v>22.0</v>
+      </c>
       <c r="N25" s="79"/>
       <c r="P25" s="0"/>
       <c r="Q25" s="0"/>
@@ -3474,21 +3518,21 @@
       <c r="I33" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="J33" s="95" t="n">
+      <c r="J33" s="95">
         <f aca="false">IF(M4="Y",SUM(J24:J32,'Page 2'!J33,'Page 3'!J33),SUM(J24:J32))</f>
-        <v>0</v>
-      </c>
-      <c r="K33" s="95" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="K33" s="95">
         <f aca="false">IF(M4="Y",SUM(K24:K32,'Page 2'!K33,'Page 3'!K33),SUM(K24:K32))</f>
-        <v>0</v>
-      </c>
-      <c r="L33" s="95" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="L33" s="95">
         <f aca="false">IF(M4="Y",SUM(L24:L32,'Page 2'!L33,'Page 3'!L33),SUM(L24:L32))</f>
-        <v>0</v>
-      </c>
-      <c r="M33" s="95" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="M33" s="95">
         <f aca="false">IF(M4="Y",SUM(M24:M32,'Page 2'!M33,'Page 3'!M33),SUM(M24:M32))</f>
-        <v>0</v>
+        <v>33.0</v>
       </c>
       <c r="N33" s="79"/>
     </row>
@@ -3556,10 +3600,16 @@
       <c r="G36" s="73"/>
       <c r="H36" s="73"/>
       <c r="I36" s="106"/>
-      <c r="J36" s="107"/>
-      <c r="K36" s="73"/>
+      <c r="J36" s="107">
+        <v>40858.0</v>
+      </c>
+      <c r="K36" s="73" t="str">
+        <v>12</v>
+      </c>
       <c r="L36" s="73"/>
-      <c r="M36" s="108"/>
+      <c r="M36" s="108">
+        <v>1233.0</v>
+      </c>
     </row>
     <row r="37" spans="1:13" customFormat="false" ht="15" hidden="false" customHeight="1" outlineLevel="0" collapsed="false">
       <c r="A37" s="102"/>
@@ -3642,7 +3692,7 @@
       <c r="L40" s="115"/>
       <c r="M40" s="116">
         <f aca="false">IF(M4="Y",SUM(M36:M39,I36:I40,'Page 2'!M40,'Page 3'!M40),SUM(M36:M39,I36:I40))</f>
-        <v>0.0</v>
+        <v>1233.0</v>
       </c>
     </row>
     <row r="41" spans="1:13" customFormat="false" ht="15.75" hidden="false" customHeight="1" outlineLevel="0" collapsed="false">

</xml_diff>